<commit_message>
Reintroduced stored proc in AwardWinnersController.  Updated project artifacts.  Queries section is pretty much good.
</commit_message>
<xml_diff>
--- a/MovieDbLite.MVC/ProjectArtifacts/CRUD-Matrix.xlsx
+++ b/MovieDbLite.MVC/ProjectArtifacts/CRUD-Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/df1cecd6e646b923/Documents/Grad_School/Databases_605_641/Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="172" documentId="8_{D94285BA-904C-4754-BEA7-FA6F49B96D4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{78C363B2-0039-4D50-9D84-F8E6576612F4}"/>
+  <xr:revisionPtr revIDLastSave="192" documentId="8_{D94285BA-904C-4754-BEA7-FA6F49B96D4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{23FB1CD5-0FCA-49C2-8AB0-A74FD85AF908}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{3E442CFB-3B9E-4565-8AFA-3418C019E055}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="74">
   <si>
     <t>F1</t>
   </si>
@@ -244,6 +244,21 @@
   </si>
   <si>
     <t>Mark Review Helpful</t>
+  </si>
+  <si>
+    <t>E19</t>
+  </si>
+  <si>
+    <t>UserRole</t>
+  </si>
+  <si>
+    <t>E20</t>
+  </si>
+  <si>
+    <t>ImageType</t>
+  </si>
+  <si>
+    <t>F15</t>
   </si>
 </sst>
 </file>
@@ -617,43 +632,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81D5C0AA-94C9-4EB9-B326-FA858FBF7415}">
-  <dimension ref="A1:AL30"/>
+  <dimension ref="A1:AO32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="U13" sqref="U13:V26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Y10" sqref="Y10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="3.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="19" width="4.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.7109375" style="1" customWidth="1"/>
+    <col min="10" max="11" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="21" width="3.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4.140625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
         <v>23</v>
@@ -709,62 +724,72 @@
       <c r="S1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="T1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="V1" s="2"/>
+      <c r="W1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:38" ht="48" x14ac:dyDescent="0.25">
+      <c r="AO1" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" ht="48" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -782,18 +807,19 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-      <c r="P2" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="P2" s="2"/>
       <c r="Q2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="R2" s="2"/>
-      <c r="S2" s="3" t="s">
+      <c r="R2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" s="2"/>
+      <c r="T2" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:38" ht="48" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" ht="48" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -817,8 +843,9 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
-    </row>
-    <row r="4" spans="1:38" ht="48" x14ac:dyDescent="0.25">
+      <c r="T3" s="2"/>
+    </row>
+    <row r="4" spans="1:41" ht="48" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -833,29 +860,30 @@
       <c r="H4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="I4" s="2"/>
+      <c r="J4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="M4" s="2"/>
+      <c r="M4" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
-      <c r="R4" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="S4" s="2"/>
-    </row>
-    <row r="5" spans="1:38" ht="48" x14ac:dyDescent="0.25">
+      <c r="R4" s="2"/>
+      <c r="S4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T4" s="2"/>
+    </row>
+    <row r="5" spans="1:41" ht="48" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -872,15 +900,16 @@
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
-      <c r="O5" s="3" t="s">
+      <c r="O5" s="2"/>
+      <c r="P5" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
-    </row>
-    <row r="6" spans="1:38" ht="48" x14ac:dyDescent="0.25">
+      <c r="T5" s="2"/>
+    </row>
+    <row r="6" spans="1:41" ht="48" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -910,8 +939,9 @@
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
-    </row>
-    <row r="7" spans="1:38" ht="48" x14ac:dyDescent="0.25">
+      <c r="T6" s="2"/>
+    </row>
+    <row r="7" spans="1:41" ht="48" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -933,10 +963,10 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -945,8 +975,9 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
-    </row>
-    <row r="8" spans="1:38" ht="48" x14ac:dyDescent="0.25">
+      <c r="T7" s="2"/>
+    </row>
+    <row r="8" spans="1:41" ht="48" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -960,22 +991,23 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="L8" s="2"/>
-      <c r="M8" s="3" t="s">
+      <c r="M8" s="2"/>
+      <c r="N8" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
-    </row>
-    <row r="9" spans="1:38" ht="48" x14ac:dyDescent="0.25">
+      <c r="T8" s="2"/>
+    </row>
+    <row r="9" spans="1:41" ht="48" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -991,22 +1023,23 @@
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
-      <c r="N9" s="3" t="s">
+      <c r="N9" s="2"/>
+      <c r="O9" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
-    </row>
-    <row r="10" spans="1:38" ht="48" x14ac:dyDescent="0.25">
+      <c r="T9" s="2"/>
+    </row>
+    <row r="10" spans="1:41" ht="48" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1018,22 +1051,23 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="3" t="s">
+      <c r="J10" s="2"/>
+      <c r="K10" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
-      <c r="P10" s="3" t="s">
+      <c r="P10" s="2"/>
+      <c r="Q10" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
-    </row>
-    <row r="11" spans="1:38" ht="48" x14ac:dyDescent="0.25">
+      <c r="T10" s="2"/>
+    </row>
+    <row r="11" spans="1:41" ht="48" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>49</v>
       </c>
@@ -1051,20 +1085,21 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
-      <c r="P11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q11" s="3" t="s">
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="R11" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="R11" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="S11" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="T11" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>50</v>
       </c>
@@ -1076,10 +1111,10 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
@@ -1088,8 +1123,9 @@
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
-    </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="T12" s="2"/>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
@@ -1104,9 +1140,7 @@
       <c r="H13" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="I13" s="2"/>
       <c r="J13" s="2" t="s">
         <v>47</v>
       </c>
@@ -1116,29 +1150,32 @@
       <c r="L13" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="M13" s="2"/>
+      <c r="M13" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
-      <c r="R13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="S13" s="2"/>
-      <c r="U13" s="1" t="s">
+      <c r="R13" s="2"/>
+      <c r="S13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="T13" s="2"/>
+      <c r="W13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="V13" s="1" t="s">
+      <c r="X13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="W13" s="1" t="s">
+      <c r="Y13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="X13" s="1" t="s">
+      <c r="Z13" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>52</v>
       </c>
@@ -1154,36 +1191,37 @@
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-      <c r="J14" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="L14" s="2"/>
-      <c r="M14" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="M14" s="2"/>
       <c r="N14" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="O14" s="2"/>
+      <c r="O14" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
-      <c r="U14" s="1" t="s">
+      <c r="T14" s="2"/>
+      <c r="W14" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="V14" s="1" t="s">
+      <c r="X14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="W14" s="1" t="s">
+      <c r="Y14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="X14" s="1" t="s">
+      <c r="Z14" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>53</v>
       </c>
@@ -1205,10 +1243,10 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-      <c r="J15" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="K15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -1217,203 +1255,229 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
-      <c r="U15" s="1" t="s">
+      <c r="T15" s="2"/>
+      <c r="W15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="V15" s="1" t="s">
+      <c r="X15" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="W15" s="1" t="s">
+      <c r="Y15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="X15" s="1" t="s">
+      <c r="Z15" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="U16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="W16" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="V16" s="1" t="s">
+      <c r="X16" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="W16" s="1" t="s">
+      <c r="Y16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="X16" s="1" t="s">
+      <c r="Z16" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U17" s="1" t="s">
+    <row r="17" spans="23:26" x14ac:dyDescent="0.25">
+      <c r="W17" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="V17" s="1" t="s">
+      <c r="X17" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="W17" s="1" t="s">
+      <c r="Y17" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="X17" s="1" t="s">
+      <c r="Z17" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U18" s="1" t="s">
+    <row r="18" spans="23:26" x14ac:dyDescent="0.25">
+      <c r="W18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="V18" s="1" t="s">
+      <c r="X18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="W18" s="1" t="s">
+      <c r="Y18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="X18" s="1" t="s">
+      <c r="Z18" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U19" s="1" t="s">
+    <row r="19" spans="23:26" x14ac:dyDescent="0.25">
+      <c r="W19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="V19" s="1" t="s">
+      <c r="X19" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="W19" s="1" t="s">
+      <c r="Y19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="X19" s="1" t="s">
+      <c r="Z19" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U20" s="1" t="s">
+    <row r="20" spans="23:26" x14ac:dyDescent="0.25">
+      <c r="W20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="V20" s="1" t="s">
+      <c r="X20" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="W20" s="1" t="s">
+      <c r="Y20" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="X20" s="1" t="s">
+      <c r="Z20" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="23:26" x14ac:dyDescent="0.25">
+      <c r="W21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X21" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z21" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="V21" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="W21" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="X21" s="1" t="s">
+    <row r="22" spans="23:26" x14ac:dyDescent="0.25">
+      <c r="W22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z22" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U22" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="V22" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="W22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="X22" s="1" t="s">
+    <row r="23" spans="23:26" x14ac:dyDescent="0.25">
+      <c r="W23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="X23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z23" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U23" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="V23" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="W23" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="X23" s="1" t="s">
+    <row r="24" spans="23:26" x14ac:dyDescent="0.25">
+      <c r="W24" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="X24" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y24" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z24" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U24" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="V24" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="W24" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="X24" s="1" t="s">
+    <row r="25" spans="23:26" x14ac:dyDescent="0.25">
+      <c r="W25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="X25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z25" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="V25" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="W25" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="X25" s="1" t="s">
+    <row r="26" spans="23:26" x14ac:dyDescent="0.25">
+      <c r="W26" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="X26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z26" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="U26" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="V26" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="W26" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X26" s="1" t="s">
+    <row r="27" spans="23:26" x14ac:dyDescent="0.25">
+      <c r="Y27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z27" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="W27" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="X27" s="1" t="s">
+    <row r="28" spans="23:26" x14ac:dyDescent="0.25">
+      <c r="Y28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z28" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="W28" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="X28" s="1" t="s">
+    <row r="29" spans="23:26" x14ac:dyDescent="0.25">
+      <c r="Y29" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z29" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="W29" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="X29" s="1" t="s">
+    <row r="30" spans="23:26" x14ac:dyDescent="0.25">
+      <c r="Y30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z30" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="21:24" x14ac:dyDescent="0.25">
-      <c r="W30" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="X30" s="1" t="s">
+    <row r="31" spans="23:26" x14ac:dyDescent="0.25">
+      <c r="Y31" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z31" s="1" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="23:26" x14ac:dyDescent="0.25">
+      <c r="Y32" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z32" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>